<commit_message>
added the rest of 21 june att
</commit_message>
<xml_diff>
--- a/Tools/Find Data for list tool.xlsx
+++ b/Tools/Find Data for list tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\preparatory\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E1B7DB-57FC-4DF3-AA34-7DCE5C6A3FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9DA4F-797B-4CF7-95A5-1DECAE55FBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6174" uniqueCount="1494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6167" uniqueCount="1488">
   <si>
     <t>ID</t>
   </si>
@@ -4541,24 +4541,6 @@
   </si>
   <si>
     <t xml:space="preserve"> بيشوي سامح</t>
-  </si>
-  <si>
-    <t>بولا عصام</t>
-  </si>
-  <si>
-    <t>بولا ملاك</t>
-  </si>
-  <si>
-    <t>كارل مينا</t>
-  </si>
-  <si>
-    <t>بولا بيشو</t>
-  </si>
-  <si>
-    <t>كيرلس ماجد ح</t>
-  </si>
-  <si>
-    <t>مينا عماد عدل</t>
   </si>
 </sst>
 </file>
@@ -4569,7 +4551,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4615,6 +4597,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4739,13 +4731,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4792,9 +4785,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4803,30 +4793,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Details" xfId="1" xr:uid="{B710E3BE-BFA5-4646-8C02-3752D9A51B63}"/>
     <cellStyle name="Normal_Sheet3" xfId="3" xr:uid="{D723C0F6-72EA-46D0-A1E3-08D55D4DC4AF}"/>
+    <cellStyle name="Normal_Table" xfId="4" xr:uid="{3825D332-5588-4FBF-BD6A-7050D961702C}"/>
   </cellStyles>
   <dxfs count="23">
     <dxf>
@@ -5064,8 +5061,8 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3215957D-A9BC-43EE-B2CB-4E112B3404E3}" name="ID" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{30E6FDFF-BAB1-49FF-A083-BC173DC93ED3}" name="الاسم" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{038FC1CE-CD64-42F1-8630-2309AD82E527}" name="الاسم2" dataDxfId="18">
-      <calculatedColumnFormula array="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],#REF!,#REF!),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{038FC1CE-CD64-42F1-8630-2309AD82E527}" name="الفصل" dataDxfId="18">
+      <calculatedColumnFormula array="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],#REF!,#REF!),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5361,18 +5358,18 @@
       <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" customWidth="1"/>
-    <col min="13" max="19" width="10.33203125" customWidth="1"/>
-    <col min="20" max="20" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="13" max="19" width="10.28515625" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5437,7 +5434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -5502,7 +5499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -5567,7 +5564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -5632,7 +5629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -5697,7 +5694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>6</v>
       </c>
@@ -5762,7 +5759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>7</v>
       </c>
@@ -5827,7 +5824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>9</v>
       </c>
@@ -5892,7 +5889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>10</v>
       </c>
@@ -5957,7 +5954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>11</v>
       </c>
@@ -6022,7 +6019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>102</v>
       </c>
@@ -6087,7 +6084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>103</v>
       </c>
@@ -6152,7 +6149,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>104</v>
       </c>
@@ -6217,7 +6214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>113</v>
       </c>
@@ -6282,7 +6279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>114</v>
       </c>
@@ -6347,7 +6344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>115</v>
       </c>
@@ -6412,7 +6409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>116</v>
       </c>
@@ -6477,7 +6474,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>118</v>
       </c>
@@ -6542,7 +6539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>119</v>
       </c>
@@ -6607,7 +6604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>120</v>
       </c>
@@ -6672,7 +6669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>121</v>
       </c>
@@ -6737,7 +6734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>122</v>
       </c>
@@ -6802,7 +6799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>123</v>
       </c>
@@ -6867,7 +6864,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>124</v>
       </c>
@@ -6932,7 +6929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>125</v>
       </c>
@@ -6997,7 +6994,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>126</v>
       </c>
@@ -7062,7 +7059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>127</v>
       </c>
@@ -7127,7 +7124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>128</v>
       </c>
@@ -7192,7 +7189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>129</v>
       </c>
@@ -7257,7 +7254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>130</v>
       </c>
@@ -7322,7 +7319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>131</v>
       </c>
@@ -7387,7 +7384,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>132</v>
       </c>
@@ -7452,7 +7449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>133</v>
       </c>
@@ -7517,7 +7514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>134</v>
       </c>
@@ -7582,7 +7579,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>135</v>
       </c>
@@ -7647,7 +7644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>136</v>
       </c>
@@ -7712,7 +7709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>137</v>
       </c>
@@ -7777,7 +7774,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>138</v>
       </c>
@@ -7842,7 +7839,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>139</v>
       </c>
@@ -7907,7 +7904,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>140</v>
       </c>
@@ -7972,7 +7969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>141</v>
       </c>
@@ -8037,7 +8034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>202</v>
       </c>
@@ -8102,7 +8099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>203</v>
       </c>
@@ -8167,7 +8164,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>204</v>
       </c>
@@ -8232,7 +8229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>210</v>
       </c>
@@ -8297,7 +8294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>211</v>
       </c>
@@ -8362,7 +8359,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>212</v>
       </c>
@@ -8427,7 +8424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>214</v>
       </c>
@@ -8492,7 +8489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>215</v>
       </c>
@@ -8557,7 +8554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>216</v>
       </c>
@@ -8622,7 +8619,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>217</v>
       </c>
@@ -8687,7 +8684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>218</v>
       </c>
@@ -8752,7 +8749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>219</v>
       </c>
@@ -8817,7 +8814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>220</v>
       </c>
@@ -8882,7 +8879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>221</v>
       </c>
@@ -8947,7 +8944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>222</v>
       </c>
@@ -9012,7 +9009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>223</v>
       </c>
@@ -9077,7 +9074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>224</v>
       </c>
@@ -9142,7 +9139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>225</v>
       </c>
@@ -9207,7 +9204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>226</v>
       </c>
@@ -9272,7 +9269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>227</v>
       </c>
@@ -9337,7 +9334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>228</v>
       </c>
@@ -9402,7 +9399,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>229</v>
       </c>
@@ -9467,7 +9464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>230</v>
       </c>
@@ -9532,7 +9529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>231</v>
       </c>
@@ -9597,7 +9594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>232</v>
       </c>
@@ -9662,7 +9659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>234</v>
       </c>
@@ -9727,7 +9724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>235</v>
       </c>
@@ -9792,7 +9789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>236</v>
       </c>
@@ -9857,7 +9854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>237</v>
       </c>
@@ -9922,7 +9919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>239</v>
       </c>
@@ -9987,7 +9984,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
         <v>240</v>
       </c>
@@ -10052,7 +10049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="12">
         <v>241</v>
       </c>
@@ -10117,7 +10114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>242</v>
       </c>
@@ -10182,7 +10179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>243</v>
       </c>
@@ -10247,7 +10244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>244</v>
       </c>
@@ -10312,7 +10309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>245</v>
       </c>
@@ -10377,7 +10374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>246</v>
       </c>
@@ -10442,7 +10439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>247</v>
       </c>
@@ -10507,7 +10504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>248</v>
       </c>
@@ -10572,7 +10569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
         <v>249</v>
       </c>
@@ -10637,7 +10634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>250</v>
       </c>
@@ -10702,7 +10699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
         <v>251</v>
       </c>
@@ -10767,7 +10764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>253</v>
       </c>
@@ -10832,7 +10829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
         <v>254</v>
       </c>
@@ -10897,7 +10894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
         <v>255</v>
       </c>
@@ -10962,7 +10959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
         <v>256</v>
       </c>
@@ -11027,7 +11024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="12">
         <v>257</v>
       </c>
@@ -11092,7 +11089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="12">
         <v>258</v>
       </c>
@@ -11157,7 +11154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
         <v>259</v>
       </c>
@@ -11222,7 +11219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
         <v>303</v>
       </c>
@@ -11287,7 +11284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>304</v>
       </c>
@@ -11352,7 +11349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>310</v>
       </c>
@@ -11417,7 +11414,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="12">
         <v>311</v>
       </c>
@@ -11482,7 +11479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="12">
         <v>312</v>
       </c>
@@ -11547,7 +11544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="12">
         <v>313</v>
       </c>
@@ -11612,7 +11609,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="12">
         <v>314</v>
       </c>
@@ -11677,7 +11674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="12">
         <v>315</v>
       </c>
@@ -11742,7 +11739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="12">
         <v>317</v>
       </c>
@@ -11807,7 +11804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="12">
         <v>318</v>
       </c>
@@ -11872,7 +11869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="12">
         <v>319</v>
       </c>
@@ -11937,7 +11934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>321</v>
       </c>
@@ -12002,7 +11999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="12">
         <v>322</v>
       </c>
@@ -12067,7 +12064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="12">
         <v>323</v>
       </c>
@@ -12132,7 +12129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="12">
         <v>324</v>
       </c>
@@ -12197,7 +12194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="12">
         <v>325</v>
       </c>
@@ -12262,7 +12259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="12">
         <v>327</v>
       </c>
@@ -12327,7 +12324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="12">
         <v>328</v>
       </c>
@@ -12392,7 +12389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="12">
         <v>329</v>
       </c>
@@ -12457,7 +12454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="12">
         <v>330</v>
       </c>
@@ -12522,7 +12519,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="12">
         <v>333</v>
       </c>
@@ -12587,7 +12584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="12">
         <v>334</v>
       </c>
@@ -12652,7 +12649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="12">
         <v>336</v>
       </c>
@@ -12717,7 +12714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="12">
         <v>337</v>
       </c>
@@ -12782,7 +12779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" s="12">
         <v>338</v>
       </c>
@@ -12847,7 +12844,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="12">
         <v>339</v>
       </c>
@@ -12912,7 +12909,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="12">
         <v>341</v>
       </c>
@@ -12977,7 +12974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="12">
         <v>342</v>
       </c>
@@ -13042,7 +13039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A119" s="12">
         <v>343</v>
       </c>
@@ -13107,7 +13104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A120" s="12">
         <v>344</v>
       </c>
@@ -13172,7 +13169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="12">
         <v>345</v>
       </c>
@@ -13237,7 +13234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="12">
         <v>346</v>
       </c>
@@ -13302,7 +13299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="12">
         <v>347</v>
       </c>
@@ -13367,7 +13364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="12">
         <v>348</v>
       </c>
@@ -13432,7 +13429,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="12">
         <v>349</v>
       </c>
@@ -13497,7 +13494,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="12">
         <v>350</v>
       </c>
@@ -13562,7 +13559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="12">
         <v>351</v>
       </c>
@@ -13627,7 +13624,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="12">
         <v>352</v>
       </c>
@@ -13692,7 +13689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="12">
         <v>402</v>
       </c>
@@ -13757,7 +13754,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="12">
         <v>403</v>
       </c>
@@ -13822,7 +13819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="12">
         <v>404</v>
       </c>
@@ -13887,7 +13884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="12">
         <v>410</v>
       </c>
@@ -13952,7 +13949,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="12">
         <v>411</v>
       </c>
@@ -14017,7 +14014,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="12">
         <v>412</v>
       </c>
@@ -14082,7 +14079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="12">
         <v>413</v>
       </c>
@@ -14147,7 +14144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="12">
         <v>415</v>
       </c>
@@ -14212,7 +14209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="12">
         <v>416</v>
       </c>
@@ -14277,7 +14274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="12">
         <v>417</v>
       </c>
@@ -14342,7 +14339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="12">
         <v>419</v>
       </c>
@@ -14407,7 +14404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="12">
         <v>420</v>
       </c>
@@ -14472,7 +14469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="12">
         <v>421</v>
       </c>
@@ -14537,7 +14534,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="12">
         <v>422</v>
       </c>
@@ -14602,7 +14599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="12">
         <v>423</v>
       </c>
@@ -14667,7 +14664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="12">
         <v>424</v>
       </c>
@@ -14732,7 +14729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="12">
         <v>426</v>
       </c>
@@ -14797,7 +14794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A146" s="12">
         <v>427</v>
       </c>
@@ -14862,7 +14859,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="12">
         <v>428</v>
       </c>
@@ -14927,7 +14924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="12">
         <v>429</v>
       </c>
@@ -14992,7 +14989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="12">
         <v>430</v>
       </c>
@@ -15057,7 +15054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A150" s="12">
         <v>431</v>
       </c>
@@ -15122,7 +15119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="12">
         <v>432</v>
       </c>
@@ -15187,7 +15184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="12">
         <v>433</v>
       </c>
@@ -15252,7 +15249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="12">
         <v>434</v>
       </c>
@@ -15317,7 +15314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="12">
         <v>435</v>
       </c>
@@ -15382,7 +15379,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="12">
         <v>436</v>
       </c>
@@ -15447,7 +15444,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="12">
         <v>437</v>
       </c>
@@ -15512,7 +15509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="12">
         <v>438</v>
       </c>
@@ -15577,7 +15574,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="12">
         <v>439</v>
       </c>
@@ -15642,7 +15639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="12">
         <v>440</v>
       </c>
@@ -15707,7 +15704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="12">
         <v>441</v>
       </c>
@@ -15772,7 +15769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="12">
         <v>442</v>
       </c>
@@ -15837,7 +15834,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="12">
         <v>443</v>
       </c>
@@ -15902,7 +15899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="12">
         <v>444</v>
       </c>
@@ -15967,7 +15964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="12">
         <v>445</v>
       </c>
@@ -16032,7 +16029,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="12">
         <v>446</v>
       </c>
@@ -16097,7 +16094,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="12">
         <v>448</v>
       </c>
@@ -16162,7 +16159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="12">
         <v>449</v>
       </c>
@@ -16227,7 +16224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="12">
         <v>450</v>
       </c>
@@ -16292,7 +16289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="12">
         <v>451</v>
       </c>
@@ -16357,7 +16354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="12">
         <v>502</v>
       </c>
@@ -16422,7 +16419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" s="12">
         <v>503</v>
       </c>
@@ -16487,7 +16484,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="12">
         <v>504</v>
       </c>
@@ -16552,7 +16549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="12">
         <v>510</v>
       </c>
@@ -16617,7 +16614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="12">
         <v>512</v>
       </c>
@@ -16682,7 +16679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" s="12">
         <v>513</v>
       </c>
@@ -16747,7 +16744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="12">
         <v>514</v>
       </c>
@@ -16812,7 +16809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="12">
         <v>515</v>
       </c>
@@ -16877,7 +16874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="12">
         <v>516</v>
       </c>
@@ -16942,7 +16939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="12">
         <v>519</v>
       </c>
@@ -17007,7 +17004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="12">
         <v>520</v>
       </c>
@@ -17072,7 +17069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="12">
         <v>521</v>
       </c>
@@ -17137,7 +17134,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="12">
         <v>523</v>
       </c>
@@ -17202,7 +17199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="12">
         <v>524</v>
       </c>
@@ -17267,7 +17264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="12">
         <v>525</v>
       </c>
@@ -17332,7 +17329,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="12">
         <v>526</v>
       </c>
@@ -17397,7 +17394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="12">
         <v>528</v>
       </c>
@@ -17462,7 +17459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="12">
         <v>529</v>
       </c>
@@ -17527,7 +17524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="12">
         <v>532</v>
       </c>
@@ -17592,7 +17589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A189" s="12">
         <v>533</v>
       </c>
@@ -17657,7 +17654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="12">
         <v>534</v>
       </c>
@@ -17722,7 +17719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="12">
         <v>602</v>
       </c>
@@ -17787,7 +17784,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="12">
         <v>603</v>
       </c>
@@ -17852,7 +17849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A193" s="12">
         <v>610</v>
       </c>
@@ -17917,7 +17914,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="12">
         <v>611</v>
       </c>
@@ -17982,7 +17979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="12">
         <v>612</v>
       </c>
@@ -18047,7 +18044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="12">
         <v>613</v>
       </c>
@@ -18112,7 +18109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A197" s="12">
         <v>614</v>
       </c>
@@ -18177,7 +18174,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="12">
         <v>615</v>
       </c>
@@ -18242,7 +18239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" s="12">
         <v>616</v>
       </c>
@@ -18307,7 +18304,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A200" s="12">
         <v>617</v>
       </c>
@@ -18372,7 +18369,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A201" s="12">
         <v>618</v>
       </c>
@@ -18437,7 +18434,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="12">
         <v>619</v>
       </c>
@@ -18502,7 +18499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A203" s="12">
         <v>620</v>
       </c>
@@ -18567,7 +18564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A204" s="12">
         <v>621</v>
       </c>
@@ -18632,7 +18629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="12">
         <v>702</v>
       </c>
@@ -18697,7 +18694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="12">
         <v>703</v>
       </c>
@@ -18762,7 +18759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="12">
         <v>710</v>
       </c>
@@ -18827,7 +18824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A208" s="12">
         <v>711</v>
       </c>
@@ -18892,7 +18889,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A209" s="12">
         <v>712</v>
       </c>
@@ -18957,7 +18954,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="12">
         <v>713</v>
       </c>
@@ -19022,7 +19019,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:21" ht="270" x14ac:dyDescent="0.25">
       <c r="A211" s="12">
         <v>714</v>
       </c>
@@ -19087,7 +19084,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A212" s="12">
         <v>715</v>
       </c>
@@ -19152,7 +19149,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="12">
         <v>716</v>
       </c>
@@ -19217,7 +19214,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A214" s="12">
         <v>717</v>
       </c>
@@ -19282,7 +19279,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A215" s="12">
         <v>718</v>
       </c>
@@ -19347,7 +19344,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" s="12">
         <v>719</v>
       </c>
@@ -19412,7 +19409,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A217" s="12">
         <v>720</v>
       </c>
@@ -19477,7 +19474,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A218" s="12">
         <v>721</v>
       </c>
@@ -19542,7 +19539,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="12">
         <v>722</v>
       </c>
@@ -19607,7 +19604,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="12">
         <v>723</v>
       </c>
@@ -19672,7 +19669,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:21" ht="345" x14ac:dyDescent="0.25">
       <c r="A221" s="12">
         <v>724</v>
       </c>
@@ -19737,7 +19734,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A222" s="12">
         <v>725</v>
       </c>
@@ -19802,7 +19799,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A223" s="12">
         <v>726</v>
       </c>
@@ -19867,7 +19864,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:21" ht="165" x14ac:dyDescent="0.25">
       <c r="A224" s="12">
         <v>727</v>
       </c>
@@ -19932,7 +19929,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:21" ht="195" x14ac:dyDescent="0.25">
       <c r="A225" s="12">
         <v>728</v>
       </c>
@@ -19997,7 +19994,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A226" s="12">
         <v>729</v>
       </c>
@@ -20062,7 +20059,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A227" s="12">
         <v>730</v>
       </c>
@@ -20127,7 +20124,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="12">
         <v>731</v>
       </c>
@@ -20192,7 +20189,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A229" s="12">
         <v>732</v>
       </c>
@@ -20257,7 +20254,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A230" s="12">
         <v>734</v>
       </c>
@@ -20322,7 +20319,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A231" s="12">
         <v>735</v>
       </c>
@@ -20387,7 +20384,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A232" s="12">
         <v>736</v>
       </c>
@@ -20452,7 +20449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A233" s="12">
         <v>737</v>
       </c>
@@ -20517,7 +20514,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="12">
         <v>738</v>
       </c>
@@ -20582,7 +20579,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A235" s="12">
         <v>739</v>
       </c>
@@ -20647,7 +20644,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="12">
         <v>740</v>
       </c>
@@ -20712,7 +20709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="12">
         <v>741</v>
       </c>
@@ -20777,7 +20774,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="12">
         <v>742</v>
       </c>
@@ -20842,7 +20839,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:21" ht="165" x14ac:dyDescent="0.25">
       <c r="A239" s="12">
         <v>743</v>
       </c>
@@ -20907,7 +20904,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="12">
         <v>744</v>
       </c>
@@ -20972,7 +20969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="12">
         <v>745</v>
       </c>
@@ -21037,7 +21034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="12">
         <v>746</v>
       </c>
@@ -21102,7 +21099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="12">
         <v>747</v>
       </c>
@@ -21167,7 +21164,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="12">
         <v>802</v>
       </c>
@@ -21232,7 +21229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="12">
         <v>803</v>
       </c>
@@ -21297,7 +21294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="12">
         <v>804</v>
       </c>
@@ -21362,7 +21359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="12">
         <v>810</v>
       </c>
@@ -21427,7 +21424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A248" s="12">
         <v>811</v>
       </c>
@@ -21492,7 +21489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="12">
         <v>812</v>
       </c>
@@ -21557,7 +21554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="12">
         <v>813</v>
       </c>
@@ -21622,7 +21619,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="12">
         <v>814</v>
       </c>
@@ -21687,7 +21684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A252" s="12">
         <v>815</v>
       </c>
@@ -21752,7 +21749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="12">
         <v>817</v>
       </c>
@@ -21817,7 +21814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="12">
         <v>818</v>
       </c>
@@ -21882,7 +21879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="12">
         <v>819</v>
       </c>
@@ -21947,7 +21944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="12">
         <v>820</v>
       </c>
@@ -22012,7 +22009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="12">
         <v>821</v>
       </c>
@@ -22077,7 +22074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="12">
         <v>822</v>
       </c>
@@ -22142,7 +22139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="12">
         <v>823</v>
       </c>
@@ -22207,7 +22204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A260" s="12">
         <v>824</v>
       </c>
@@ -22272,7 +22269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A261" s="12">
         <v>825</v>
       </c>
@@ -22337,7 +22334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A262" s="12">
         <v>826</v>
       </c>
@@ -22402,7 +22399,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="12">
         <v>828</v>
       </c>
@@ -22467,7 +22464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A264" s="12">
         <v>829</v>
       </c>
@@ -22532,7 +22529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A265" s="12">
         <v>830</v>
       </c>
@@ -22597,7 +22594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A266" s="12">
         <v>831</v>
       </c>
@@ -22662,7 +22659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="12">
         <v>833</v>
       </c>
@@ -22727,7 +22724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="12">
         <v>835</v>
       </c>
@@ -22792,7 +22789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A269" s="12">
         <v>836</v>
       </c>
@@ -22857,7 +22854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="12">
         <v>837</v>
       </c>
@@ -22922,7 +22919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="12">
         <v>838</v>
       </c>
@@ -22987,7 +22984,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="12">
         <v>839</v>
       </c>
@@ -23052,7 +23049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="12">
         <v>840</v>
       </c>
@@ -23117,7 +23114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="12">
         <v>841</v>
       </c>
@@ -23182,7 +23179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A275" s="12">
         <v>842</v>
       </c>
@@ -23247,7 +23244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="12">
         <v>843</v>
       </c>
@@ -23312,7 +23309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A277" s="12">
         <v>844</v>
       </c>
@@ -23377,7 +23374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A278" s="12">
         <v>845</v>
       </c>
@@ -23442,7 +23439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="12">
         <v>846</v>
       </c>
@@ -23507,7 +23504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A280" s="12">
         <v>847</v>
       </c>
@@ -23572,7 +23569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" s="12">
         <v>848</v>
       </c>
@@ -23637,7 +23634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A282" s="12">
         <v>849</v>
       </c>
@@ -23702,7 +23699,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A283" s="12">
         <v>850</v>
       </c>
@@ -23767,7 +23764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="12">
         <v>851</v>
       </c>
@@ -23832,7 +23829,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A285" s="12">
         <v>853</v>
       </c>
@@ -23897,7 +23894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="12">
         <v>854</v>
       </c>
@@ -23962,7 +23959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="12">
         <v>855</v>
       </c>
@@ -24027,7 +24024,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A288" s="12">
         <v>856</v>
       </c>
@@ -24092,7 +24089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A289" s="12">
         <v>859</v>
       </c>
@@ -24157,7 +24154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A290" s="12">
         <v>860</v>
       </c>
@@ -24222,7 +24219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" s="12">
         <v>862</v>
       </c>
@@ -24287,7 +24284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A292" s="12">
         <v>863</v>
       </c>
@@ -24352,7 +24349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A293" s="12">
         <v>864</v>
       </c>
@@ -24417,7 +24414,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="12">
         <v>865</v>
       </c>
@@ -24482,7 +24479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="12">
         <v>866</v>
       </c>
@@ -24547,7 +24544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A296" s="12">
         <v>867</v>
       </c>
@@ -24612,7 +24609,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="12">
         <v>868</v>
       </c>
@@ -24677,7 +24674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A298" s="12">
         <v>869</v>
       </c>
@@ -24742,7 +24739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" s="12">
         <v>870</v>
       </c>
@@ -24807,7 +24804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A300" s="12">
         <v>871</v>
       </c>
@@ -24872,7 +24869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A301" s="12">
         <v>872</v>
       </c>
@@ -24937,7 +24934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A302" s="12">
         <v>873</v>
       </c>
@@ -25002,7 +24999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A303" s="12">
         <v>874</v>
       </c>
@@ -25067,7 +25064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A304" s="12">
         <v>875</v>
       </c>
@@ -25132,7 +25129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A305" s="12">
         <v>876</v>
       </c>
@@ -25197,7 +25194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A306" s="12">
         <v>877</v>
       </c>
@@ -25262,7 +25259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A307" s="12">
         <v>878</v>
       </c>
@@ -25327,7 +25324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="12">
         <v>879</v>
       </c>
@@ -25392,7 +25389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="309" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A309" s="12">
         <v>880</v>
       </c>
@@ -25457,7 +25454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="310" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="12">
         <v>881</v>
       </c>
@@ -25522,7 +25519,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A311" s="12">
         <v>882</v>
       </c>
@@ -25587,7 +25584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A312" s="12">
         <v>883</v>
       </c>
@@ -25652,7 +25649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A313" s="12">
         <v>884</v>
       </c>
@@ -25717,7 +25714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A314" s="12">
         <v>886</v>
       </c>
@@ -25782,7 +25779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A315" s="12">
         <v>887</v>
       </c>
@@ -25847,7 +25844,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A316" s="12">
         <v>888</v>
       </c>
@@ -25912,7 +25909,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A317" s="12">
         <v>889</v>
       </c>
@@ -25977,7 +25974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A318" s="12">
         <v>890</v>
       </c>
@@ -26042,7 +26039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A319" s="12">
         <v>891</v>
       </c>
@@ -26107,7 +26104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A320" s="12">
         <v>892</v>
       </c>
@@ -26172,7 +26169,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A321" s="12">
         <v>893</v>
       </c>
@@ -26237,7 +26234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A322" s="12">
         <v>894</v>
       </c>
@@ -26302,7 +26299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="323" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A323" s="12">
         <v>900</v>
       </c>
@@ -26382,81 +26379,81 @@
   </sheetPr>
   <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" customWidth="1"/>
-    <col min="27" max="27" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1359</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1369</v>
+        <v>1361</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1368</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
-        <v>418</v>
-      </c>
-      <c r="B2" s="28"/>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="33">
+        <v>140</v>
+      </c>
+      <c r="B2" s="27"/>
       <c r="C2" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C2" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>not found</v>
+        <f t="array" aca="1" ref="C2" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس متى الرسول</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
-        <v>530</v>
-      </c>
-      <c r="B3" s="28"/>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>116</v>
+      </c>
+      <c r="B3" s="27"/>
       <c r="C3" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C3" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>not found</v>
+        <f t="array" aca="1" ref="C3" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس متى الرسول</v>
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
-        <v>210</v>
-      </c>
-      <c r="B4" s="28"/>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>443</v>
+      </c>
+      <c r="B4" s="27"/>
       <c r="C4" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C4" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">ابرام جرجس سعيد </v>
+        <f t="array" aca="1" ref="C4" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس يوحنا الرسول</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
-        <v>532</v>
-      </c>
-      <c r="B5" s="28"/>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>448</v>
+      </c>
+      <c r="B5" s="27"/>
       <c r="C5" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C5" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>ارساني عماد وليم</v>
+        <f t="array" aca="1" ref="C5" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس يوحنا الرسول</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -26468,14 +26465,14 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
-        <v>115</v>
-      </c>
-      <c r="B6" s="28"/>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
+        <v>333</v>
+      </c>
+      <c r="B6" s="27"/>
       <c r="C6" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بافلي سامر سمير</v>
+        <f t="array" aca="1" ref="C6" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس لوقا الرسول</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -26487,14 +26484,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
-        <v>137</v>
-      </c>
-      <c r="B7" s="28"/>
+    <row r="7" spans="1:30" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>874</v>
+      </c>
+      <c r="B7" s="27"/>
       <c r="C7" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C7" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بافلي عماد لمعي توماس</v>
+        <f t="array" aca="1" ref="C7" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس بولس الرسول</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -26506,14 +26503,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
-        <v>873</v>
-      </c>
-      <c r="B8" s="28"/>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>856</v>
+      </c>
+      <c r="B8" s="27"/>
       <c r="C8" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C8" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بافلي كمال رزق الله</v>
+        <f t="array" aca="1" ref="C8" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس بولس الرسول</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISNUMBER(FIND("/",TEXT($D2,"#"))),"/","-")</f>
@@ -26526,14 +26523,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="28" t="s">
-        <v>1491</v>
-      </c>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>214</v>
+      </c>
+      <c r="B9" s="27"/>
       <c r="C9" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C9" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بولا بيشوي جمال</v>
+        <f t="array" aca="1" ref="C9" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس مرقس الرسول</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -26547,14 +26544,14 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="2"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="28" t="s">
-        <v>1488</v>
-      </c>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>120</v>
+      </c>
+      <c r="B10" s="27"/>
       <c r="C10" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C10" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بولا عصام عبده كامل</v>
+        <f t="array" aca="1" ref="C10" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس متى الرسول</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -26568,14 +26565,14 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="4"/>
     </row>
-    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="28" t="s">
-        <v>1489</v>
-      </c>
+    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <v>873</v>
+      </c>
+      <c r="B11" s="27"/>
       <c r="C11" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C11" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بولا ملاك لمعي</v>
+        <f t="array" aca="1" ref="C11" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس بولس الرسول</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>1363</v>
@@ -26586,14 +26583,14 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="2"/>
     </row>
-    <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
-        <v>214</v>
-      </c>
-      <c r="B12" s="23"/>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>345</v>
+      </c>
+      <c r="B12" s="22"/>
       <c r="C12" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C12" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">بولا هاني جرجس </v>
+        <f t="array" aca="1" ref="C12" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس لوقا الرسول</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -26607,14 +26604,14 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="4"/>
     </row>
-    <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
-        <v>818</v>
-      </c>
-      <c r="B13" s="28"/>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>846</v>
+      </c>
+      <c r="B13" s="27"/>
       <c r="C13" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C13" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">بيشوي جمال صدقي </v>
+        <f t="array" aca="1" ref="C13" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس بولس الرسول</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -26628,14 +26625,14 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="2"/>
     </row>
-    <row r="14" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>819</v>
-      </c>
-      <c r="B14" s="21"/>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>855</v>
+      </c>
+      <c r="B14" s="20"/>
       <c r="C14" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C14" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">بيير جوزيف مكرم </v>
+        <f t="array" aca="1" ref="C14" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس بولس الرسول</v>
       </c>
       <c r="Z14" s="1" t="s">
         <v>1353</v>
@@ -26646,16 +26643,16 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="4"/>
     </row>
-    <row r="15" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
-        <v>218</v>
-      </c>
-      <c r="B15" s="23"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <v>422</v>
+      </c>
+      <c r="B15" s="22"/>
       <c r="C15" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C15" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>توماس ايهاب سمير سامي</v>
-      </c>
-      <c r="D15" s="21"/>
+        <f t="array" aca="1" ref="C15" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس يوحنا الرسول</v>
+      </c>
+      <c r="D15" s="20"/>
       <c r="Z15" s="3" t="s">
         <v>1367</v>
       </c>
@@ -26665,14 +26662,14 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="2"/>
     </row>
-    <row r="16" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
-        <v>122</v>
-      </c>
-      <c r="B16" s="30"/>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>247</v>
+      </c>
+      <c r="B16" s="29"/>
       <c r="C16" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C16" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>توماس ايهاب سمير شحاته</v>
+        <f t="array" aca="1" ref="C16" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس مرقس الرسول</v>
       </c>
       <c r="Z16" t="s">
         <v>1370</v>
@@ -26683,25 +26680,25 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="4"/>
     </row>
-    <row r="17" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
-        <v>219</v>
-      </c>
-      <c r="B17" s="30"/>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>318</v>
+      </c>
+      <c r="B17" s="29"/>
       <c r="C17" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C17" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">جاستن محب يوسف </v>
+        <f t="array" aca="1" ref="C17" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس لوقا الرسول</v>
       </c>
       <c r="AC17" s="1"/>
       <c r="AD17" s="2"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
-        <v>323</v>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>444</v>
       </c>
       <c r="C18" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C18" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>جون اسحق سمير</v>
+        <f t="array" aca="1" ref="C18" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس يوحنا الرسول</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -26709,390 +26706,319 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="4"/>
     </row>
-    <row r="19" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
-        <v>251</v>
-      </c>
-      <c r="B19" s="29"/>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <v>435</v>
+      </c>
+      <c r="B19" s="28"/>
       <c r="C19" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C19" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>حبيب ايهاب</v>
-      </c>
-      <c r="D19" s="21">
+        <f t="array" aca="1" ref="C19" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>القديس يوحنا الرسول</v>
+      </c>
+      <c r="D19" s="20">
         <v>1</v>
       </c>
       <c r="AC19" s="1"/>
       <c r="AD19" s="2"/>
     </row>
-    <row r="20" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
-        <v>224</v>
-      </c>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
       <c r="C20" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C20" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>ديفيد رامي مجدي</v>
+        <f t="array" aca="1" ref="C20" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
-        <v>427</v>
-      </c>
-      <c r="B21" s="31"/>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C21" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>ديفيد صبحي صبحي</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
-        <v>125</v>
-      </c>
-      <c r="B22" s="30"/>
+        <f t="array" aca="1" ref="C21" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>ديفيد لطفي تادرس</v>
+        <f t="array" aca="1" ref="C22" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
-        <v>126</v>
-      </c>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
       <c r="C23" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C23" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>ريمون شفيق سمير</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="15">
-        <v>870</v>
-      </c>
-      <c r="B24" s="29"/>
+        <f t="array" aca="1" ref="C23" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C24" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>ستيفن اشرف عزيز</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="17">
-        <v>515</v>
-      </c>
+        <f t="array" aca="1" ref="C24" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
       <c r="C25" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C25" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">شارل شريف مكرم </v>
+        <f t="array" aca="1" ref="C25" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="C26" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C26" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>فادي فارس عبد الاحد</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
-        <v>436</v>
-      </c>
-      <c r="B27" s="29"/>
+        <f t="array" aca="1" ref="C26" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C27" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">فيكتور عاطف وديع </v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="19">
-        <v>874</v>
-      </c>
-      <c r="B28" s="30"/>
+        <f t="array" aca="1" ref="C27" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C28" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">فيلوباتير جورج صمؤيل </v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="16">
-        <v>229</v>
-      </c>
-      <c r="B29" s="22"/>
+        <f t="array" aca="1" ref="C28" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C29" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">فيلوباتير روماني برسوم </v>
+        <f t="array" aca="1" ref="C29" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="18">
-        <v>229</v>
-      </c>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
       <c r="C30" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C30" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">فيلوباتير روماني برسوم </v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" t="s">
-        <v>1490</v>
-      </c>
+        <f t="array" aca="1" ref="C30" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
       <c r="C31" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C31" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">كارل مينا عادل </v>
+        <f t="array" aca="1" ref="C31" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="15">
-        <v>836</v>
-      </c>
-      <c r="B32" s="29"/>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C32" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">كيرلس رفعت فرنساوي </v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="17">
-        <v>138</v>
-      </c>
-      <c r="B33" s="28"/>
+        <f t="array" aca="1" ref="C32" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C33" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>كيرلس روماني امين ‏ حبيب</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="24">
-        <v>253</v>
-      </c>
+        <f t="array" aca="1" ref="C33" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
       <c r="C34" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C34" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>كيرلس فايق ماهر</v>
+        <f t="array" aca="1" ref="C34" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="17">
-        <v>839</v>
-      </c>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
       <c r="C35" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C35" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">كيرلس كمال كامل </v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
-        <v>234</v>
-      </c>
-      <c r="B36" s="30"/>
+        <f t="array" aca="1" ref="C35" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C36" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">كيرلس ماجد حلمي </v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+        <f t="array" aca="1" ref="C36" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
-      <c r="B37" t="s">
-        <v>1492</v>
-      </c>
       <c r="C37" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C37" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">كيرلس ماجد حلمي </v>
+        <f t="array" aca="1" ref="C37" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="19">
-        <v>846</v>
-      </c>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
       <c r="C38" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C38" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">مارك دانيال لبيب </v>
+        <f t="array" aca="1" ref="C38" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>333</v>
-      </c>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C39" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C39" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>مارك ميلاد فكري</v>
+        <f t="array" aca="1" ref="C39" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="25">
-        <v>130</v>
-      </c>
-      <c r="B40" s="29"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C40" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>مارك وجدي فكري</v>
+        <f t="array" aca="1" ref="C40" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="27">
-        <v>240</v>
-      </c>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
       <c r="C41" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C41" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">ماركو اشرف ابراهيم </v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="25">
-        <v>242</v>
-      </c>
-      <c r="B42" s="29"/>
+        <f t="array" aca="1" ref="C41" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C42" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>مينا رافت حلمي</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="25">
-        <v>448</v>
-      </c>
+        <f t="array" aca="1" ref="C42" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
       <c r="C43" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C43" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">مينا رفعت شحاته </v>
+        <f t="array" aca="1" ref="C43" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="27">
-        <v>448</v>
-      </c>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
       <c r="C44" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C44" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">مينا رفعت شحاته </v>
+        <f t="array" aca="1" ref="C44" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>190</v>
-      </c>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C45" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C45" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>مينا عاطف داوود</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>1493</v>
-      </c>
+        <f t="array" aca="1" ref="C45" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C46" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C46" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>مينا عماد عدلي</v>
+        <f t="array" aca="1" ref="C46" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="25">
-        <v>867</v>
-      </c>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
       <c r="C47" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C47" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>مينا ماجد ايوب</v>
+        <f t="array" aca="1" ref="C47" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="25">
-        <v>892</v>
-      </c>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
       <c r="C48" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C48" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>يوسف الامير جمال</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="19">
-        <v>247</v>
-      </c>
+        <f t="array" aca="1" ref="C48" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
       <c r="C49" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C49" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>يوسف جيمي ادور</v>
+        <f t="array" aca="1" ref="C49" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="18">
-        <v>881</v>
-      </c>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
       <c r="C50" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C50" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">يوسف ريمون فؤاد </v>
+        <f t="array" aca="1" ref="C50" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A51" s="18">
-        <v>719</v>
-      </c>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
       <c r="C51" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C51" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>بيشوي ملاك فوزي</v>
+        <f t="array" aca="1" ref="C51" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="18">
-        <v>446</v>
-      </c>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
       <c r="C52" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C52" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v xml:space="preserve">مايكل سامي جابر </v>
+        <f t="array" aca="1" ref="C52" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="32">
-        <v>140</v>
-      </c>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="C53" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C53" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الاسم2]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>يوسف سامح جميل</v>
+        <f t="array" aca="1" ref="C53" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>الخدام</v>
       </c>
       <c r="D53">
         <v>1</v>

</xml_diff>

<commit_message>
some queries for the conference
</commit_message>
<xml_diff>
--- a/Tools/Find Data for list tool.xlsx
+++ b/Tools/Find Data for list tool.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\preparatory\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9DA4F-797B-4CF7-95A5-1DECAE55FBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF0D2E5-A6EC-4623-8594-B551F39F86CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4551,7 +4551,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4602,14 +4602,22 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4634,8 +4642,20 @@
         <bgColor theme="9" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -4730,6 +4750,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4738,7 +4788,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4814,8 +4864,20 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -5061,8 +5123,8 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3215957D-A9BC-43EE-B2CB-4E112B3404E3}" name="ID" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{30E6FDFF-BAB1-49FF-A083-BC173DC93ED3}" name="الاسم" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{038FC1CE-CD64-42F1-8630-2309AD82E527}" name="الفصل" dataDxfId="18">
-      <calculatedColumnFormula array="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],#REF!,#REF!),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{038FC1CE-CD64-42F1-8630-2309AD82E527}" name="تاريخ الميلاد" dataDxfId="18">
+      <calculatedColumnFormula array="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],#REF!,#REF!),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -26380,7 +26442,7 @@
   <dimension ref="A1:AD53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26395,7 +26457,7 @@
     <col min="27" max="27" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -26403,57 +26465,57 @@
         <v>1359</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1368</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
-        <v>140</v>
+    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34">
+        <v>417</v>
       </c>
       <c r="B2" s="27"/>
-      <c r="C2" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C2" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس متى الرسول</v>
+      <c r="C2" s="7" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39643</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
-        <v>116</v>
+    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="35">
+        <v>892</v>
       </c>
       <c r="B3" s="27"/>
-      <c r="C3" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C3" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس متى الرسول</v>
+      <c r="C3" s="7" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39824</v>
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
-        <v>443</v>
+    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35">
+        <v>881</v>
       </c>
       <c r="B4" s="27"/>
-      <c r="C4" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C4" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس يوحنا الرسول</v>
+      <c r="C4" s="7" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39750</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
-        <v>448</v>
+    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35">
+        <v>880</v>
       </c>
       <c r="B5" s="27"/>
-      <c r="C5" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C5" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس يوحنا الرسول</v>
+      <c r="C5" s="7" cm="1">
+        <f t="array" aca="1" ref="C5" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>40007</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -26465,14 +26527,14 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
-        <v>333</v>
+    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35">
+        <v>869</v>
       </c>
       <c r="B6" s="27"/>
-      <c r="C6" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس لوقا الرسول</v>
+      <c r="C6" s="7" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39357</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -26484,14 +26546,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
-        <v>874</v>
+    <row r="7" spans="1:30" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35">
+        <v>245</v>
       </c>
       <c r="B7" s="27"/>
-      <c r="C7" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C7" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس بولس الرسول</v>
+      <c r="C7" s="7" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39914</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -26503,14 +26565,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
-        <v>856</v>
+    <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36">
+        <v>884</v>
       </c>
       <c r="B8" s="27"/>
-      <c r="C8" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C8" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس بولس الرسول</v>
+      <c r="C8" s="7" cm="1">
+        <f t="array" aca="1" ref="C8" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39743</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISNUMBER(FIND("/",TEXT($D2,"#"))),"/","-")</f>
@@ -26523,14 +26585,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
-        <v>214</v>
+    <row r="9" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35">
+        <v>878</v>
       </c>
       <c r="B9" s="27"/>
-      <c r="C9" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C9" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس مرقس الرسول</v>
+      <c r="C9" s="7" cm="1">
+        <f t="array" aca="1" ref="C9" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39878</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -26544,14 +26606,14 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="2"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="33">
-        <v>120</v>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35">
+        <v>722</v>
       </c>
       <c r="B10" s="27"/>
-      <c r="C10" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C10" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس متى الرسول</v>
+      <c r="C10" s="7" cm="1">
+        <f t="array" aca="1" ref="C10" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39711</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -26565,14 +26627,14 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="4"/>
     </row>
-    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
-        <v>873</v>
+    <row r="11" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="35">
+        <v>515</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C11" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس بولس الرسول</v>
+      <c r="C11" s="7" cm="1">
+        <f t="array" aca="1" ref="C11" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39986</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>1363</v>
@@ -26583,14 +26645,12 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="2"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
-        <v>345</v>
-      </c>
+    <row r="12" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="37"/>
       <c r="B12" s="22"/>
-      <c r="C12" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C12" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس لوقا الرسول</v>
+      <c r="C12" s="7" cm="1">
+        <f t="array" aca="1" ref="C12" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -26604,14 +26664,14 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="4"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
-        <v>846</v>
+    <row r="13" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="35">
+        <v>128</v>
       </c>
       <c r="B13" s="27"/>
-      <c r="C13" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C13" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس بولس الرسول</v>
+      <c r="C13" s="7" cm="1">
+        <f t="array" aca="1" ref="C13" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>39640</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -26626,13 +26686,11 @@
       <c r="AD13" s="2"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
-        <v>855</v>
-      </c>
+      <c r="A14" s="33"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C14" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس بولس الرسول</v>
+      <c r="C14" s="7" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="Z14" s="1" t="s">
         <v>1353</v>
@@ -26644,13 +26702,11 @@
       <c r="AD14" s="4"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
-        <v>422</v>
-      </c>
+      <c r="A15" s="33"/>
       <c r="B15" s="22"/>
-      <c r="C15" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C15" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس يوحنا الرسول</v>
+      <c r="C15" s="7" cm="1">
+        <f t="array" aca="1" ref="C15" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D15" s="20"/>
       <c r="Z15" s="3" t="s">
@@ -26663,13 +26719,11 @@
       <c r="AD15" s="2"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
-        <v>247</v>
-      </c>
+      <c r="A16" s="33"/>
       <c r="B16" s="29"/>
-      <c r="C16" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C16" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس مرقس الرسول</v>
+      <c r="C16" s="7" cm="1">
+        <f t="array" aca="1" ref="C16" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="Z16" t="s">
         <v>1370</v>
@@ -26681,24 +26735,20 @@
       <c r="AD16" s="4"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="33">
-        <v>318</v>
-      </c>
+      <c r="A17" s="33"/>
       <c r="B17" s="29"/>
-      <c r="C17" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C17" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس لوقا الرسول</v>
+      <c r="C17" s="7" cm="1">
+        <f t="array" aca="1" ref="C17" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="AC17" s="1"/>
       <c r="AD17" s="2"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
-        <v>444</v>
-      </c>
-      <c r="C18" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C18" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس يوحنا الرسول</v>
+      <c r="A18" s="33"/>
+      <c r="C18" s="7" cm="1">
+        <f t="array" aca="1" ref="C18" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -26707,13 +26757,11 @@
       <c r="AD18" s="4"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
-        <v>435</v>
-      </c>
+      <c r="A19" s="33"/>
       <c r="B19" s="28"/>
-      <c r="C19" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C19" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>القديس يوحنا الرسول</v>
+      <c r="C19" s="7" cm="1">
+        <f t="array" aca="1" ref="C19" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D19" s="20">
         <v>1</v>
@@ -26723,9 +26771,9 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
-      <c r="C20" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C20" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C20" s="7" cm="1">
+        <f t="array" aca="1" ref="C20" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -26734,17 +26782,17 @@
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="30"/>
-      <c r="C21" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C21" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C21" s="7" cm="1">
+        <f t="array" aca="1" ref="C21" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="29"/>
-      <c r="C22" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C22" s="7" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -26752,24 +26800,24 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
-      <c r="C23" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C23" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C23" s="7" cm="1">
+        <f t="array" aca="1" ref="C23" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="28"/>
-      <c r="C24" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C24" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C24" s="7" cm="1">
+        <f t="array" aca="1" ref="C24" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
-      <c r="C25" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C25" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C25" s="7" cm="1">
+        <f t="array" aca="1" ref="C25" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -26777,33 +26825,33 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
-      <c r="C26" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C26" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C26" s="7" cm="1">
+        <f t="array" aca="1" ref="C26" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="28"/>
-      <c r="C27" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C27" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C27" s="7" cm="1">
+        <f t="array" aca="1" ref="C27" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="29"/>
-      <c r="C28" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C28" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C28" s="7" cm="1">
+        <f t="array" aca="1" ref="C28" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="21"/>
-      <c r="C29" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C29" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C29" s="7" cm="1">
+        <f t="array" aca="1" ref="C29" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -26811,16 +26859,16 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
-      <c r="C30" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C30" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C30" s="7" cm="1">
+        <f t="array" aca="1" ref="C30" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
-      <c r="C31" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C31" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C31" s="7" cm="1">
+        <f t="array" aca="1" ref="C31" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -26829,24 +26877,24 @@
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="28"/>
-      <c r="C32" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C32" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C32" s="7" cm="1">
+        <f t="array" aca="1" ref="C32" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="27"/>
-      <c r="C33" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C33" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C33" s="7" cm="1">
+        <f t="array" aca="1" ref="C33" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
-      <c r="C34" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C34" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C34" s="7" cm="1">
+        <f t="array" aca="1" ref="C34" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -26854,24 +26902,24 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
-      <c r="C35" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C35" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C35" s="7" cm="1">
+        <f t="array" aca="1" ref="C35" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="29"/>
-      <c r="C36" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C36" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C36" s="7" cm="1">
+        <f t="array" aca="1" ref="C36" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
-      <c r="C37" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C37" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C37" s="7" cm="1">
+        <f t="array" aca="1" ref="C37" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -26879,18 +26927,18 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
-      <c r="C38" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C38" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C38" s="7" cm="1">
+        <f t="array" aca="1" ref="C38" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C39" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C39" s="7" cm="1">
+        <f t="array" aca="1" ref="C39" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -26899,9 +26947,9 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="28"/>
-      <c r="C40" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C40" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C40" s="7" cm="1">
+        <f t="array" aca="1" ref="C40" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -26909,24 +26957,24 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
-      <c r="C41" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C41" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C41" s="7" cm="1">
+        <f t="array" aca="1" ref="C41" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="28"/>
-      <c r="C42" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C42" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C42" s="7" cm="1">
+        <f t="array" aca="1" ref="C42" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
-      <c r="C43" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C43" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C43" s="7" cm="1">
+        <f t="array" aca="1" ref="C43" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -26934,24 +26982,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="26"/>
-      <c r="C44" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C44" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C44" s="7" cm="1">
+        <f t="array" aca="1" ref="C44" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C45" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C45" s="7" cm="1">
+        <f t="array" aca="1" ref="C45" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C46" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C46" s="7" cm="1">
+        <f t="array" aca="1" ref="C46" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -26959,9 +27007,9 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
-      <c r="C47" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C47" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C47" s="7" cm="1">
+        <f t="array" aca="1" ref="C47" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -26969,16 +27017,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
-      <c r="C48" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C48" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C48" s="7" cm="1">
+        <f t="array" aca="1" ref="C48" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
-      <c r="C49" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C49" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C49" s="7" cm="1">
+        <f t="array" aca="1" ref="C49" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -26986,9 +27034,9 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
-      <c r="C50" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C50" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C50" s="7" cm="1">
+        <f t="array" aca="1" ref="C50" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -26996,9 +27044,9 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
-      <c r="C51" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C51" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C51" s="7" cm="1">
+        <f t="array" aca="1" ref="C51" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -27006,9 +27054,9 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
-      <c r="C52" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C52" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C52" s="7" cm="1">
+        <f t="array" aca="1" ref="C52" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -27016,9 +27064,9 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
-      <c r="C53" s="7" t="str" cm="1">
-        <f t="array" aca="1" ref="C53" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[الفصل]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
-        <v>الخدام</v>
+      <c r="C53" s="7" cm="1">
+        <f t="array" aca="1" ref="C53" ca="1">_xlfn.XLOOKUP(IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table4[[#This Row],[ID]],Table4[[#This Row],[الاسم]]&amp;"*"),IF(Table4[[#This Row],[ID]]&lt;&gt;"",Table1[ID],Table1[fname]),INDIRECT(_xlfn.TEXTJOIN(,TRUE,"Table1[",_xlfn.XLOOKUP(Table4[[#Headers],[تاريخ الميلاد]],Table2[Name],Table2[Tag]),"]")),"not found",IF(Table4[[#This Row],[ID]]&lt;&gt;"",0,2))</f>
+        <v>33920</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -27097,9 +27145,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>